<commit_message>
fix spelling error and add some constraints
</commit_message>
<xml_diff>
--- a/New_Diet/service.xlsx
+++ b/New_Diet/service.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FIT5120\New_Diet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2989C55E-0F58-44E5-8B6C-703E064CDBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4FDC54-3E6E-45DE-84E7-B124C0DCC16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22176" windowHeight="13176" xr2:uid="{82B47A94-5358-4183-84D1-6953A77FD95A}"/>
   </bookViews>
@@ -41,12 +41,6 @@
     <t>Fruit</t>
   </si>
   <si>
-    <t>Vegetable</t>
-  </si>
-  <si>
-    <t>Meat</t>
-  </si>
-  <si>
     <t>Food</t>
   </si>
   <si>
@@ -59,9 +53,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>Grain</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dairy </t>
   </si>
   <si>
@@ -69,6 +60,15 @@
   </si>
   <si>
     <t>Serving</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Grains</t>
+  </si>
+  <si>
+    <t>Vegetables</t>
   </si>
 </sst>
 </file>
@@ -464,31 +464,31 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -499,62 +499,62 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2">
         <v>4.5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
         <v>2.5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
         <v>3.5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>2.5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -565,51 +565,51 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2">
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1">
         <v>2.5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>